<commit_message>
Append of Edit Test Case
</commit_message>
<xml_diff>
--- a/data/TC4.xlsx
+++ b/data/TC4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -57,7 +57,10 @@
     <t>10002</t>
   </si>
   <si>
-    <t>10005</t>
+    <t>DemoLeadA</t>
+  </si>
+  <si>
+    <t>DemoLeadB</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,8 @@
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -457,10 +461,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates for delete lead
</commit_message>
<xml_diff>
--- a/data/TC4.xlsx
+++ b/data/TC4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Username</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>DemoLeadB</t>
+  </si>
+  <si>
+    <t>kavitha padmanaban</t>
+  </si>
+  <si>
+    <t>padmanaban,kavitha</t>
+  </si>
+  <si>
+    <t>Govindaraju,Prabhu</t>
+  </si>
+  <si>
+    <t>prabhu Govindaraju</t>
   </si>
 </sst>
 </file>
@@ -415,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -509,12 +521,41 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="E6:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>261611</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>546896</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>